<commit_message>
Ahora las materias se obtienen de una base de datos(MongoDB) Se optimizo el programa
</commit_message>
<xml_diff>
--- a/Simulacion.xlsx
+++ b/Simulacion.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="103">
   <si>
     <t>Aulas</t>
   </si>
@@ -178,142 +178,151 @@
     <t>UNIFICADAS 3/4</t>
   </si>
   <si>
+    <t>Introducción a la Informática</t>
+  </si>
+  <si>
+    <t>Marketing I</t>
+  </si>
+  <si>
+    <t>Metodología del Diseño</t>
+  </si>
+  <si>
+    <t>Informática</t>
+  </si>
+  <si>
+    <t>Contabilidad I</t>
+  </si>
+  <si>
+    <t>Introducción a la Publicidad</t>
+  </si>
+  <si>
+    <t>Morfología</t>
+  </si>
+  <si>
+    <t>Economía I</t>
+  </si>
+  <si>
+    <t>Matemática Discreta</t>
+  </si>
+  <si>
+    <t>Sistemas Económicos</t>
+  </si>
+  <si>
+    <t>Taller de Escritura y Oratoria</t>
+  </si>
+  <si>
+    <t>Física I</t>
+  </si>
+  <si>
+    <t>Teorías de la comunicación</t>
+  </si>
+  <si>
+    <t>Lingüística</t>
+  </si>
+  <si>
+    <t>Derecho Civil y Comercial</t>
+  </si>
+  <si>
+    <t>Antropología Cultural y Regional</t>
+  </si>
+  <si>
+    <t>Análisis Matemático l</t>
+  </si>
+  <si>
     <t>Neurofisiologia</t>
   </si>
   <si>
+    <t>Taller de Diseño Gráfico I</t>
+  </si>
+  <si>
+    <t>Taller de Alfabetización académica</t>
+  </si>
+  <si>
+    <t>Análisis Matemático I</t>
+  </si>
+  <si>
+    <t>Programación Estructurada</t>
+  </si>
+  <si>
+    <t>Diseño y Animación 2D</t>
+  </si>
+  <si>
+    <t>Historia del Arte y del Diseño</t>
+  </si>
+  <si>
+    <t>Química Inorgánica</t>
+  </si>
+  <si>
+    <t>Sistemas y Organizaciones</t>
+  </si>
+  <si>
+    <t>Informática Aplicada al Diseño I</t>
+  </si>
+  <si>
+    <t>Álgebra</t>
+  </si>
+  <si>
+    <t>Neurodesarrollo</t>
+  </si>
+  <si>
+    <t>Introducción al Pensamiento Filosófico y Científico</t>
+  </si>
+  <si>
+    <t>Fundamento de Economía</t>
+  </si>
+  <si>
+    <t>Estrategias y Modelos de Negocios</t>
+  </si>
+  <si>
+    <t>Arquitectura de Computadoras</t>
+  </si>
+  <si>
+    <t>Introducción al Diseño de Indumentaria y textil</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Programación I</t>
+  </si>
+  <si>
+    <t>Morfología I</t>
+  </si>
+  <si>
     <t>Introducción a la Moldería</t>
   </si>
   <si>
-    <t>Álgebra y Lógica Computacional</t>
-  </si>
-  <si>
-    <t>Morfología</t>
-  </si>
-  <si>
-    <t>Teorías de la comunicación</t>
-  </si>
-  <si>
-    <t>Psicología General I</t>
-  </si>
-  <si>
-    <t>Contabilidad I</t>
-  </si>
-  <si>
-    <t>Introducción a la Informática</t>
-  </si>
-  <si>
-    <t>Historia Epistemológica de la Psicología</t>
-  </si>
-  <si>
-    <t>Introducción a la Publicidad</t>
-  </si>
-  <si>
-    <t>Introducción al Derecho Civil y Comercial</t>
-  </si>
-  <si>
-    <t>Comunicación</t>
-  </si>
-  <si>
-    <t>Geometría Computacional II</t>
-  </si>
-  <si>
-    <t>Física I</t>
-  </si>
-  <si>
-    <t>Psicología General II</t>
-  </si>
-  <si>
-    <t>Informática</t>
-  </si>
-  <si>
-    <t>Taller de Producción Publicitaria Gráfica I</t>
-  </si>
-  <si>
-    <t>Computación I</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Programación I</t>
-  </si>
-  <si>
-    <t>Inglés I</t>
-  </si>
-  <si>
-    <t>Psicología General</t>
-  </si>
-  <si>
-    <t>Matemática Aplicada a la Nutrición</t>
-  </si>
-  <si>
-    <t>Taller de Alfabetización académica</t>
-  </si>
-  <si>
-    <t>Historia del Arte y del Diseño</t>
-  </si>
-  <si>
-    <t>Programación Estructurada</t>
-  </si>
-  <si>
-    <t>Fundamentos de Contabilidad</t>
-  </si>
-  <si>
-    <t>Química General</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Informática </t>
-  </si>
-  <si>
-    <t>Fundamento de Economía</t>
-  </si>
-  <si>
-    <t>Análisis Matemático I</t>
-  </si>
-  <si>
-    <t>Anatomia y Fisiología de los Sistemas</t>
+    <t xml:space="preserve">Programación II </t>
+  </si>
+  <si>
+    <t>Computación II</t>
+  </si>
+  <si>
+    <t>Neurociencias II</t>
+  </si>
+  <si>
+    <t>Bioquímica</t>
+  </si>
+  <si>
+    <t>Geometría Computacional I</t>
   </si>
   <si>
     <t>Instituciones del Derecho Romano</t>
   </si>
   <si>
-    <t>Sistemas Económicos</t>
-  </si>
-  <si>
-    <t>Neurociencias I</t>
-  </si>
-  <si>
-    <t>Morfología I</t>
-  </si>
-  <si>
-    <t>Antropología</t>
-  </si>
-  <si>
-    <t>Informática I</t>
-  </si>
-  <si>
-    <t>Lingüística</t>
-  </si>
-  <si>
-    <t>Principios de Economía Política</t>
-  </si>
-  <si>
-    <t>Sistemas y Organizaciones</t>
-  </si>
-  <si>
-    <t>Neurodesarrollo</t>
-  </si>
-  <si>
-    <t>Estadística</t>
-  </si>
-  <si>
-    <t>Fundamentos de Sociología</t>
-  </si>
-  <si>
-    <t>Antropología Cultural y Regional</t>
-  </si>
-  <si>
-    <t>Introducción a las Ciencias Jurídicas</t>
-  </si>
-  <si>
-    <t>Anatomía y Fisiología General</t>
+    <t>Introducción a la Tipografía</t>
+  </si>
+  <si>
+    <t>Teoría de la Administración</t>
+  </si>
+  <si>
+    <t>Antropología Cultural</t>
+  </si>
+  <si>
+    <t>Introducción a la Psicopedagogía</t>
+  </si>
+  <si>
+    <t>Historia Económica</t>
+  </si>
+  <si>
+    <t>Anatomía</t>
   </si>
 </sst>
 </file>
@@ -734,17 +743,17 @@
       <c r="G2" t="s">
         <v>54</v>
       </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" t="b">
-        <v>0</v>
+      <c r="H2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1032,22 +1041,22 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
@@ -1067,22 +1076,22 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F12" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G12" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
@@ -1189,17 +1198,17 @@
       <c r="G15" t="s">
         <v>66</v>
       </c>
-      <c r="H15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" t="b">
-        <v>0</v>
+      <c r="H15" t="s">
+        <v>99</v>
+      </c>
+      <c r="I15" t="s">
+        <v>99</v>
+      </c>
+      <c r="J15" t="s">
+        <v>99</v>
+      </c>
+      <c r="K15" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1224,17 +1233,17 @@
       <c r="G16" t="s">
         <v>67</v>
       </c>
-      <c r="H16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" t="b">
-        <v>0</v>
-      </c>
-      <c r="K16" t="b">
-        <v>0</v>
+      <c r="H16" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" t="s">
+        <v>100</v>
+      </c>
+      <c r="J16" t="s">
+        <v>100</v>
+      </c>
+      <c r="K16" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1254,22 +1263,22 @@
         <v>68</v>
       </c>
       <c r="F17" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="G17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17" t="b">
-        <v>0</v>
-      </c>
-      <c r="K17" t="b">
-        <v>0</v>
+        <v>94</v>
+      </c>
+      <c r="H17" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" t="s">
+        <v>94</v>
+      </c>
+      <c r="J17" t="s">
+        <v>94</v>
+      </c>
+      <c r="K17" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1289,22 +1298,22 @@
         <v>69</v>
       </c>
       <c r="F18" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="G18" t="s">
-        <v>69</v>
-      </c>
-      <c r="H18" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K18" t="b">
-        <v>0</v>
+        <v>95</v>
+      </c>
+      <c r="H18" t="s">
+        <v>95</v>
+      </c>
+      <c r="I18" t="s">
+        <v>95</v>
+      </c>
+      <c r="J18" t="s">
+        <v>95</v>
+      </c>
+      <c r="K18" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1312,34 +1321,34 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="F19" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="G19" t="s">
-        <v>70</v>
-      </c>
-      <c r="H19" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" t="b">
-        <v>0</v>
-      </c>
-      <c r="K19" t="b">
-        <v>0</v>
+        <v>96</v>
+      </c>
+      <c r="H19" t="s">
+        <v>96</v>
+      </c>
+      <c r="I19" t="s">
+        <v>96</v>
+      </c>
+      <c r="J19" t="s">
+        <v>96</v>
+      </c>
+      <c r="K19" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1347,22 +1356,22 @@
         <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H20" t="b">
         <v>0</v>
@@ -1382,22 +1391,22 @@
         <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H21" t="b">
         <v>0</v>
@@ -1417,22 +1426,22 @@
         <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H22" t="b">
         <v>0</v>
@@ -1452,22 +1461,22 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H23" t="b">
         <v>0</v>
@@ -1487,22 +1496,22 @@
         <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H24" t="b">
         <v>0</v>
@@ -1522,22 +1531,22 @@
         <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H25" t="b">
         <v>0</v>
@@ -1557,22 +1566,22 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H26" t="b">
         <v>0</v>
@@ -1592,22 +1601,22 @@
         <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H27" t="b">
         <v>0</v>
@@ -1627,34 +1636,34 @@
         <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G28" t="s">
-        <v>79</v>
-      </c>
-      <c r="H28" t="s">
-        <v>69</v>
-      </c>
-      <c r="I28" t="s">
-        <v>69</v>
-      </c>
-      <c r="J28" t="s">
-        <v>69</v>
-      </c>
-      <c r="K28" t="s">
-        <v>69</v>
+        <v>78</v>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K28" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1662,22 +1671,22 @@
         <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H29" t="b">
         <v>0</v>
@@ -1697,34 +1706,34 @@
         <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F30" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="G30" t="s">
-        <v>94</v>
-      </c>
-      <c r="H30" t="s">
-        <v>94</v>
-      </c>
-      <c r="I30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J30" t="s">
-        <v>94</v>
-      </c>
-      <c r="K30" t="s">
-        <v>94</v>
+        <v>80</v>
+      </c>
+      <c r="H30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K30" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1732,22 +1741,22 @@
         <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H31" t="b">
         <v>0</v>
@@ -1767,34 +1776,34 @@
         <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="D32" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="E32" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="F32" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="G32" t="s">
-        <v>83</v>
-      </c>
-      <c r="H32" t="s">
-        <v>97</v>
-      </c>
-      <c r="I32" t="s">
-        <v>97</v>
-      </c>
-      <c r="J32" t="s">
-        <v>97</v>
-      </c>
-      <c r="K32" t="s">
-        <v>97</v>
+        <v>56</v>
+      </c>
+      <c r="H32" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" t="b">
+        <v>0</v>
+      </c>
+      <c r="J32" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1802,22 +1811,22 @@
         <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H33" t="b">
         <v>0</v>
@@ -1837,34 +1846,34 @@
         <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G34" t="s">
-        <v>85</v>
-      </c>
-      <c r="H34" t="s">
-        <v>98</v>
-      </c>
-      <c r="I34" t="s">
-        <v>98</v>
-      </c>
-      <c r="J34" t="s">
-        <v>98</v>
-      </c>
-      <c r="K34" t="s">
-        <v>98</v>
+        <v>83</v>
+      </c>
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" t="b">
+        <v>0</v>
+      </c>
+      <c r="J34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -1872,22 +1881,22 @@
         <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H35" t="b">
         <v>0</v>
@@ -1907,22 +1916,22 @@
         <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H36" t="b">
         <v>0</v>
@@ -1942,34 +1951,34 @@
         <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F37" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G37" t="s">
-        <v>95</v>
-      </c>
-      <c r="H37" t="s">
-        <v>95</v>
-      </c>
-      <c r="I37" t="s">
-        <v>95</v>
-      </c>
-      <c r="J37" t="s">
-        <v>95</v>
-      </c>
-      <c r="K37" t="s">
-        <v>95</v>
+        <v>86</v>
+      </c>
+      <c r="H37" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" t="b">
+        <v>0</v>
+      </c>
+      <c r="J37" t="b">
+        <v>0</v>
+      </c>
+      <c r="K37" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -1977,22 +1986,22 @@
         <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H38" t="b">
         <v>0</v>
@@ -2012,22 +2021,22 @@
         <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C39" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D39" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E39" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F39" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G39" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H39" t="b">
         <v>0</v>
@@ -2047,34 +2056,34 @@
         <v>49</v>
       </c>
       <c r="B40" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="C40" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="D40" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="E40" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="F40" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G40" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H40" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I40" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J40" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K40" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -2082,34 +2091,34 @@
         <v>50</v>
       </c>
       <c r="B41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G41" t="s">
-        <v>91</v>
-      </c>
-      <c r="H41" t="b">
-        <v>0</v>
-      </c>
-      <c r="I41" t="b">
-        <v>0</v>
-      </c>
-      <c r="J41" t="b">
-        <v>0</v>
-      </c>
-      <c r="K41" t="b">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="H41" t="s">
+        <v>101</v>
+      </c>
+      <c r="I41" t="s">
+        <v>101</v>
+      </c>
+      <c r="J41" t="s">
+        <v>101</v>
+      </c>
+      <c r="K41" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -2117,34 +2126,34 @@
         <v>51</v>
       </c>
       <c r="B42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G42" t="s">
-        <v>92</v>
-      </c>
-      <c r="H42" t="b">
-        <v>0</v>
-      </c>
-      <c r="I42" t="b">
-        <v>0</v>
-      </c>
-      <c r="J42" t="b">
-        <v>0</v>
-      </c>
-      <c r="K42" t="b">
-        <v>0</v>
+        <v>91</v>
+      </c>
+      <c r="H42" t="s">
+        <v>102</v>
+      </c>
+      <c r="I42" t="s">
+        <v>102</v>
+      </c>
+      <c r="J42" t="s">
+        <v>102</v>
+      </c>
+      <c r="K42" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -2152,34 +2161,34 @@
         <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G43" t="s">
-        <v>93</v>
-      </c>
-      <c r="H43" t="s">
-        <v>99</v>
-      </c>
-      <c r="I43" t="s">
-        <v>99</v>
-      </c>
-      <c r="J43" t="s">
-        <v>99</v>
-      </c>
-      <c r="K43" t="s">
-        <v>99</v>
+        <v>92</v>
+      </c>
+      <c r="H43" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" t="b">
+        <v>0</v>
+      </c>
+      <c r="J43" t="b">
+        <v>0</v>
+      </c>
+      <c r="K43" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -2187,22 +2196,22 @@
         <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="D44" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="E44" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="F44" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="G44" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="H44" t="b">
         <v>0</v>

</xml_diff>